<commit_message>
Add comments for excel gen
And update generated assessments
</commit_message>
<xml_diff>
--- a/assessments/FinOps++/assessment.xlsx
+++ b/assessments/FinOps++/assessment.xlsx
@@ -551,12 +551,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -860,1478 +859,1480 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/113.md", "113")</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/114.md", "114")</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/115.md", "115")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/116.md", "116")</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/117.md", "117")</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/097.md", "097")</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/098.md", "098")</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/099.md", "099")</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/100.md", "100")</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/101.md", "101")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/091.md", "091")</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/092.md", "092")</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/093.md", "093")</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/094.md", "094")</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/095.md", "095")</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/096.md", "096")</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/124.md", "124")</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/125.md", "125")</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/126.md", "126")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/127.md", "127")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/128.md", "128")</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/129.md", "129")</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/130.md", "130")</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/131.md", "131")</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/132.md", "132")</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/133.md", "133")</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/134.md", "134")</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/107.md", "107")</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/108.md", "108")</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/109.md", "109")</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/110.md", "110")</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/111.md", "111")</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/112.md", "112")</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3" t="s">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/118.md", "118")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/119.md", "119")</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/120.md", "120")</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3" t="s">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/121.md", "121")</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3" t="s">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/122.md", "122")</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/123.md", "123")</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/061.md", "061")</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3" t="s">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/062.md", "062")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3" t="s">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/063.md", "063")</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3" t="s">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/064.md", "064")</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/065.md", "065")</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3" t="s">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/066.md", "066")</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/073.md", "073")</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3" t="s">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/074.md", "074")</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3" t="s">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/075.md", "075")</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3" t="s">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/076.md", "076")</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3" t="s">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/077.md", "077")</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3" t="s">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/078.md", "078")</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3" t="s">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/079.md", "079")</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3" t="s">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/080.md", "080")</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3" t="s">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/081.md", "081")</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3" t="s">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/082.md", "082")</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3" t="s">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/083.md", "083")</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3" t="s">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/084.md", "084")</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3" t="s">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/067.md", "067")</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3" t="s">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/068.md", "068")</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3" t="s">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/069.md", "069")</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3" t="s">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/070.md", "070")</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/071.md", "071")</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3" t="s">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/072.md", "072")</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3" t="s">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/009.md", "009")</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3" t="s">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/010.md", "010")</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3" t="s">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/011.md", "011")</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3" t="s">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/012.md", "012")</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3" t="s">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/013.md", "013")</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3" t="s">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/014.md", "014")</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3" t="s">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/015.md", "015")</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3" t="s">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/023.md", "023")</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3" t="s">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/024.md", "024")</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3" t="s">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/025.md", "025")</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3" t="s">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/026.md", "026")</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3" t="s">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/027.md", "027")</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3" t="s">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/028.md", "028")</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3" t="s">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/029.md", "029")</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3" t="s">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/001.md", "001")</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3" t="s">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/002.md", "002")</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3" t="s">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/003.md", "003")</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3" t="s">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/004.md", "004")</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3" t="s">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/005.md", "005")</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3" t="s">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/006.md", "006")</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3" t="s">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/007.md", "007")</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3" t="s">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/008.md", "008")</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3" t="s">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/016.md", "016")</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3" t="s">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/017.md", "017")</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3" t="s">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/018.md", "018")</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3" t="s">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/019.md", "019")</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3" t="s">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/020.md", "020")</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3" t="s">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/021.md", "021")</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3" t="s">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/022.md", "022")</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/049.md", "049")</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3" t="s">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D95" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/050.md", "050")</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3" t="s">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D96" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/051.md", "051")</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3" t="s">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/052.md", "052")</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3" t="s">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D98" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/053.md", "053")</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3" t="s">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/054.md", "054")</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3" t="s">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D100" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/043.md", "043")</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3" t="s">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/044.md", "044")</f>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3" t="s">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D102" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/045.md", "045")</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3" t="s">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D103" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/046.md", "046")</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3" t="s">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D104" s="2">
+      <c r="D104" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/047.md", "047")</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3" t="s">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D105" s="2">
+      <c r="D105" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/048.md", "048")</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3" t="s">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D106" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/037.md", "037")</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3" t="s">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D107" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/038.md", "038")</f>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="3"/>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3" t="s">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D108" s="2">
+      <c r="D108" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/039.md", "039")</f>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3" t="s">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D109" s="2">
+      <c r="D109" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/040.md", "040")</f>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3" t="s">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D110" s="2">
+      <c r="D110" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/041.md", "041")</f>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="3"/>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3" t="s">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D111" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/042.md", "042")</f>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="3"/>
-      <c r="B112" s="3" t="s">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/030.md", "030")</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3" t="s">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D113" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/031.md", "031")</f>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="3"/>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3" t="s">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D114" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/032.md", "032")</f>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3" t="s">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D115" s="2">
+      <c r="D115" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/033.md", "033")</f>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3" t="s">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D116" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/034.md", "034")</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3" t="s">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D117" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/035.md", "035")</f>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3" t="s">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D118" s="2">
+      <c r="D118" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/036.md", "036")</f>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3" t="s">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D119" s="2">
+      <c r="D119" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/055.md", "055")</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3" t="s">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D120" s="2">
+      <c r="D120" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/056.md", "056")</f>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3" t="s">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D121" s="2">
+      <c r="D121" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/057.md", "057")</f>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3" t="s">
+      <c r="A122" s="2"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D122" s="2">
+      <c r="D122" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/058.md", "058")</f>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3" t="s">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D123" s="2">
+      <c r="D123" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/059.md", "059")</f>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3" t="s">
+      <c r="A124" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D124" s="2">
+      <c r="D124" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/060.md", "060")</f>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C125" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D125" s="2">
+      <c r="D125" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/102.md", "102")</f>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3" t="s">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D126" s="2">
+      <c r="D126" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/103.md", "103")</f>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="3"/>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3" t="s">
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D127" s="2">
+      <c r="D127" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/104.md", "104")</f>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="3"/>
-      <c r="B128" s="3"/>
-      <c r="C128" s="3" t="s">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D128" s="2">
+      <c r="D128" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/105.md", "105")</f>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="3"/>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3" t="s">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D129" s="2">
+      <c r="D129" s="1">
         <f>HYPERLINK("https://github.com/FinOpsPP/Framework-Assessment/tree/main/components/actions/106.md", "106")</f>
         <v>0</v>
       </c>

</xml_diff>